<commit_message>
tuple to list, theory doc
</commit_message>
<xml_diff>
--- a/mitchell10x3.xlsx
+++ b/mitchell10x3.xlsx
@@ -568,12 +568,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Name 40</t>
+          <t>Name 44</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Name 33</t>
+          <t>Name 46</t>
         </is>
       </c>
       <c r="D8" s="4">
@@ -591,12 +591,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Name 61</t>
+          <t>Name 49</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Name 69</t>
+          <t>Name 36</t>
         </is>
       </c>
       <c r="D9" s="4">
@@ -614,12 +614,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Name 28</t>
+          <t>Name 54</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Name 43</t>
+          <t>Name 23</t>
         </is>
       </c>
       <c r="D10" s="4">
@@ -637,12 +637,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Name 81</t>
+          <t>Name 19</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Name 71</t>
+          <t>Name 72</t>
         </is>
       </c>
       <c r="D11" s="4">
@@ -660,12 +660,12 @@
       </c>
       <c r="B12" s="7" t="inlineStr">
         <is>
-          <t>Name 84</t>
+          <t>Name 58</t>
         </is>
       </c>
       <c r="C12" s="7" t="inlineStr">
         <is>
-          <t>Name 79</t>
+          <t>Name 83</t>
         </is>
       </c>
       <c r="D12" s="8">
@@ -716,12 +716,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Name 55</t>
+          <t>Name 52</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Name 27</t>
+          <t>Name 46</t>
         </is>
       </c>
       <c r="D16" s="4">
@@ -739,12 +739,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Name 47</t>
+          <t>Name 61</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Name 27</t>
+          <t>Name 36</t>
         </is>
       </c>
       <c r="D17" s="4">
@@ -762,12 +762,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Name 77</t>
+          <t>Name 36</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Name 39</t>
+          <t>Name 69</t>
         </is>
       </c>
       <c r="D18" s="4">
@@ -785,12 +785,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Name 51</t>
+          <t>Name 33</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Name 89</t>
+          <t>Name 38</t>
         </is>
       </c>
       <c r="D19" s="4">
@@ -808,12 +808,12 @@
       </c>
       <c r="B20" s="7" t="inlineStr">
         <is>
+          <t>Name 48</t>
+        </is>
+      </c>
+      <c r="C20" s="7" t="inlineStr">
+        <is>
           <t>Name 18</t>
-        </is>
-      </c>
-      <c r="C20" s="7" t="inlineStr">
-        <is>
-          <t>Name 77</t>
         </is>
       </c>
       <c r="D20" s="8">
@@ -11555,6 +11555,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="J3" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="15" t="n"/>
@@ -11568,6 +11571,9 @@
           <t>NS</t>
         </is>
       </c>
+      <c r="J4" t="n">
+        <v>410</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="19" t="n"/>
@@ -11585,7 +11591,9 @@
       <c r="H5" s="7" t="n"/>
       <c r="I5" s="7" t="n"/>
       <c r="J5" s="7" t="n"/>
-      <c r="K5" s="7" t="n"/>
+      <c r="K5" s="7" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="15" t="n">
@@ -11604,6 +11612,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="J6" t="n">
+        <v>620</v>
       </c>
     </row>
     <row r="7">
@@ -11618,6 +11629,9 @@
           <t>NS</t>
         </is>
       </c>
+      <c r="K7" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="19" t="n"/>
@@ -11634,7 +11648,9 @@
       <c r="G8" s="7" t="n"/>
       <c r="H8" s="7" t="n"/>
       <c r="I8" s="7" t="n"/>
-      <c r="J8" s="7" t="n"/>
+      <c r="J8" s="7" t="n">
+        <v>300</v>
+      </c>
       <c r="K8" s="7" t="n"/>
     </row>
     <row r="9">
@@ -11654,6 +11670,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="J9" t="n">
+        <v>280</v>
       </c>
     </row>
     <row r="10">
@@ -11668,6 +11687,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="J10" t="n">
+        <v>230</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="19" t="n"/>
@@ -11685,7 +11707,9 @@
       <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
       <c r="J11" s="7" t="n"/>
-      <c r="K11" s="7" t="n"/>
+      <c r="K11" s="7" t="n">
+        <v>520</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" s="15" t="n">
@@ -11703,6 +11727,16 @@
       <c r="F12" s="15" t="inlineStr">
         <is>
           <t>Both</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Avg</t>
         </is>
       </c>
     </row>
@@ -11718,6 +11752,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="K13" t="n">
+        <v>220</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="19" t="n"/>
@@ -11735,7 +11772,9 @@
       <c r="H14" s="7" t="n"/>
       <c r="I14" s="7" t="n"/>
       <c r="J14" s="7" t="n"/>
-      <c r="K14" s="7" t="n"/>
+      <c r="K14" s="7" t="n">
+        <v>600</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="15" t="n">
@@ -11754,6 +11793,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="J15" t="n">
+        <v>760</v>
       </c>
     </row>
     <row r="16">
@@ -11767,6 +11809,9 @@
         <is>
           <t>None</t>
         </is>
+      </c>
+      <c r="K16" t="n">
+        <v>730</v>
       </c>
     </row>
     <row r="17">
@@ -11785,7 +11830,9 @@
       <c r="G17" s="7" t="n"/>
       <c r="H17" s="7" t="n"/>
       <c r="I17" s="7" t="n"/>
-      <c r="J17" s="7" t="n"/>
+      <c r="J17" s="7" t="n">
+        <v>760</v>
+      </c>
       <c r="K17" s="7" t="n"/>
     </row>
     <row r="18">
@@ -11808,6 +11855,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="J18" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="19">
@@ -11822,6 +11872,16 @@
           <t>NS</t>
         </is>
       </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="19" t="n"/>
@@ -11838,7 +11898,9 @@
       <c r="G20" s="7" t="n"/>
       <c r="H20" s="7" t="n"/>
       <c r="I20" s="7" t="n"/>
-      <c r="J20" s="7" t="n"/>
+      <c r="J20" s="7" t="n">
+        <v>770</v>
+      </c>
       <c r="K20" s="7" t="n"/>
     </row>
     <row r="21">
@@ -11858,6 +11920,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="K21" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="22">
@@ -11872,6 +11937,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="K22" t="n">
+        <v>560</v>
+      </c>
     </row>
     <row r="23">
       <c r="B23" s="19" t="n"/>
@@ -11889,7 +11957,9 @@
       <c r="H23" s="7" t="n"/>
       <c r="I23" s="7" t="n"/>
       <c r="J23" s="7" t="n"/>
-      <c r="K23" s="7" t="n"/>
+      <c r="K23" s="7" t="n">
+        <v>770</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" s="15" t="n">
@@ -11908,6 +11978,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="K24" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="25">
@@ -11922,6 +11995,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="K25" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" s="19" t="n"/>
@@ -11939,7 +12015,9 @@
       <c r="H26" s="7" t="n"/>
       <c r="I26" s="7" t="n"/>
       <c r="J26" s="7" t="n"/>
-      <c r="K26" s="7" t="n"/>
+      <c r="K26" s="7" t="n">
+        <v>660</v>
+      </c>
     </row>
     <row r="27">
       <c r="B27" s="15" t="n">
@@ -11958,6 +12036,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="K27" t="n">
+        <v>370</v>
       </c>
     </row>
     <row r="28">
@@ -11972,6 +12053,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="K28" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="19" t="n"/>
@@ -11989,7 +12073,9 @@
       <c r="H29" s="7" t="n"/>
       <c r="I29" s="7" t="n"/>
       <c r="J29" s="7" t="n"/>
-      <c r="K29" s="7" t="n"/>
+      <c r="K29" s="7" t="n">
+        <v>430</v>
+      </c>
     </row>
     <row r="30">
       <c r="B30" s="15" t="n">
@@ -12008,6 +12094,9 @@
         <is>
           <t>None</t>
         </is>
+      </c>
+      <c r="K30" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="31">
@@ -12021,6 +12110,9 @@
         <is>
           <t>NS</t>
         </is>
+      </c>
+      <c r="K31" t="n">
+        <v>330</v>
       </c>
     </row>
     <row r="32">
@@ -12040,7 +12132,9 @@
       <c r="H32" s="7" t="n"/>
       <c r="I32" s="7" t="n"/>
       <c r="J32" s="7" t="n"/>
-      <c r="K32" s="7" t="n"/>
+      <c r="K32" s="7" t="n">
+        <v>270</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="15" t="n">
@@ -12062,6 +12156,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="K33" t="n">
+        <v>780</v>
       </c>
     </row>
     <row r="34">
@@ -12076,6 +12173,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="J34" t="n">
+        <v>770</v>
+      </c>
     </row>
     <row r="35">
       <c r="B35" s="19" t="n"/>
@@ -12092,7 +12192,9 @@
       <c r="G35" s="7" t="n"/>
       <c r="H35" s="7" t="n"/>
       <c r="I35" s="7" t="n"/>
-      <c r="J35" s="7" t="n"/>
+      <c r="J35" s="7" t="n">
+        <v>390</v>
+      </c>
       <c r="K35" s="7" t="n"/>
     </row>
     <row r="36">
@@ -12112,6 +12214,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="J36" t="n">
+        <v>460</v>
       </c>
     </row>
     <row r="37">
@@ -12126,6 +12231,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="K37" t="n">
+        <v>590</v>
+      </c>
     </row>
     <row r="38">
       <c r="B38" s="19" t="n"/>
@@ -12143,7 +12251,9 @@
       <c r="H38" s="7" t="n"/>
       <c r="I38" s="7" t="n"/>
       <c r="J38" s="7" t="n"/>
-      <c r="K38" s="7" t="n"/>
+      <c r="K38" s="7" t="n">
+        <v>750</v>
+      </c>
     </row>
     <row r="39">
       <c r="B39" s="15" t="n">
@@ -12162,6 +12272,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="K39" t="n">
+        <v>640</v>
       </c>
     </row>
     <row r="40">
@@ -12176,6 +12289,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="J40" t="n">
+        <v>460</v>
+      </c>
     </row>
     <row r="41">
       <c r="B41" s="19" t="n"/>
@@ -12193,7 +12309,9 @@
       <c r="H41" s="7" t="n"/>
       <c r="I41" s="7" t="n"/>
       <c r="J41" s="7" t="n"/>
-      <c r="K41" s="7" t="n"/>
+      <c r="K41" s="7" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="42">
       <c r="B42" s="15" t="n">
@@ -12212,6 +12330,9 @@
         <is>
           <t>None</t>
         </is>
+      </c>
+      <c r="K42" t="n">
+        <v>490</v>
       </c>
     </row>
     <row r="43">
@@ -12226,6 +12347,9 @@
           <t>NS</t>
         </is>
       </c>
+      <c r="J43" t="n">
+        <v>570</v>
+      </c>
     </row>
     <row r="44">
       <c r="B44" s="19" t="n"/>
@@ -12243,7 +12367,9 @@
       <c r="H44" s="7" t="n"/>
       <c r="I44" s="7" t="n"/>
       <c r="J44" s="7" t="n"/>
-      <c r="K44" s="7" t="n"/>
+      <c r="K44" s="7" t="n">
+        <v>360</v>
+      </c>
     </row>
     <row r="45">
       <c r="B45" s="15" t="n">
@@ -12262,6 +12388,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="J45" t="n">
+        <v>530</v>
       </c>
     </row>
     <row r="46">
@@ -12274,6 +12403,16 @@
       <c r="F46" s="15" t="inlineStr">
         <is>
           <t>NS</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Avg</t>
         </is>
       </c>
     </row>
@@ -12294,7 +12433,9 @@
       <c r="H47" s="7" t="n"/>
       <c r="I47" s="7" t="n"/>
       <c r="J47" s="7" t="n"/>
-      <c r="K47" s="7" t="n"/>
+      <c r="K47" s="7" t="n">
+        <v>280</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="15" t="n">
@@ -12316,6 +12457,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="J48" t="n">
+        <v>260</v>
       </c>
     </row>
     <row r="49">
@@ -12330,6 +12474,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="J49" t="n">
+        <v>420</v>
+      </c>
     </row>
     <row r="50">
       <c r="B50" s="19" t="n"/>
@@ -12347,7 +12494,9 @@
       <c r="H50" s="7" t="n"/>
       <c r="I50" s="7" t="n"/>
       <c r="J50" s="7" t="n"/>
-      <c r="K50" s="7" t="n"/>
+      <c r="K50" s="7" t="n">
+        <v>700</v>
+      </c>
     </row>
     <row r="51">
       <c r="B51" s="15" t="n">
@@ -12366,6 +12515,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="K51" t="n">
+        <v>310</v>
       </c>
     </row>
     <row r="52">
@@ -12380,6 +12532,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="J52" t="n">
+        <v>720</v>
+      </c>
     </row>
     <row r="53">
       <c r="B53" s="19" t="n"/>
@@ -12397,7 +12552,9 @@
       <c r="H53" s="7" t="n"/>
       <c r="I53" s="7" t="n"/>
       <c r="J53" s="7" t="n"/>
-      <c r="K53" s="7" t="n"/>
+      <c r="K53" s="7" t="n">
+        <v>270</v>
+      </c>
     </row>
     <row r="54">
       <c r="B54" s="15" t="n">
@@ -12415,6 +12572,16 @@
       <c r="F54" s="15" t="inlineStr">
         <is>
           <t>None</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Avg</t>
         </is>
       </c>
     </row>
@@ -12430,6 +12597,9 @@
           <t>NS</t>
         </is>
       </c>
+      <c r="K55" t="n">
+        <v>700</v>
+      </c>
     </row>
     <row r="56">
       <c r="B56" s="19" t="n"/>
@@ -12447,7 +12617,9 @@
       <c r="H56" s="7" t="n"/>
       <c r="I56" s="7" t="n"/>
       <c r="J56" s="7" t="n"/>
-      <c r="K56" s="7" t="n"/>
+      <c r="K56" s="7" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="57">
       <c r="B57" s="15" t="n">
@@ -12466,6 +12638,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="J57" t="n">
+        <v>260</v>
       </c>
     </row>
     <row r="58">
@@ -12480,6 +12655,9 @@
           <t>NS</t>
         </is>
       </c>
+      <c r="J58" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="59">
       <c r="B59" s="19" t="n"/>
@@ -12496,8 +12674,16 @@
       <c r="G59" s="7" t="n"/>
       <c r="H59" s="7" t="n"/>
       <c r="I59" s="7" t="n"/>
-      <c r="J59" s="7" t="n"/>
-      <c r="K59" s="7" t="n"/>
+      <c r="J59" s="7" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
+      <c r="K59" s="7" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="B60" s="15" t="n">
@@ -12516,6 +12702,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="K60" t="n">
+        <v>190</v>
       </c>
     </row>
     <row r="61">
@@ -12528,6 +12717,16 @@
       <c r="F61" s="15" t="inlineStr">
         <is>
           <t>None</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Avg</t>
         </is>
       </c>
     </row>
@@ -12547,7 +12746,9 @@
       <c r="G62" s="7" t="n"/>
       <c r="H62" s="7" t="n"/>
       <c r="I62" s="7" t="n"/>
-      <c r="J62" s="7" t="n"/>
+      <c r="J62" s="7" t="n">
+        <v>170</v>
+      </c>
       <c r="K62" s="7" t="n"/>
     </row>
     <row r="63">
@@ -12570,6 +12771,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="K63" t="n">
+        <v>380</v>
       </c>
     </row>
     <row r="64">
@@ -12584,6 +12788,9 @@
           <t>None</t>
         </is>
       </c>
+      <c r="J64" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="65">
       <c r="B65" s="19" t="n"/>
@@ -12601,7 +12808,9 @@
       <c r="H65" s="7" t="n"/>
       <c r="I65" s="7" t="n"/>
       <c r="J65" s="7" t="n"/>
-      <c r="K65" s="7" t="n"/>
+      <c r="K65" s="7" t="n">
+        <v>160</v>
+      </c>
     </row>
     <row r="66">
       <c r="B66" s="15" t="n">
@@ -12620,6 +12829,9 @@
         <is>
           <t>None</t>
         </is>
+      </c>
+      <c r="J66" t="n">
+        <v>610</v>
       </c>
     </row>
     <row r="67">
@@ -12634,6 +12846,9 @@
           <t>NS</t>
         </is>
       </c>
+      <c r="K67" t="n">
+        <v>380</v>
+      </c>
     </row>
     <row r="68">
       <c r="B68" s="19" t="n"/>
@@ -12651,7 +12866,9 @@
       <c r="H68" s="7" t="n"/>
       <c r="I68" s="7" t="n"/>
       <c r="J68" s="7" t="n"/>
-      <c r="K68" s="7" t="n"/>
+      <c r="K68" s="7" t="n">
+        <v>620</v>
+      </c>
     </row>
     <row r="69">
       <c r="B69" s="15" t="n">
@@ -12669,6 +12886,16 @@
       <c r="F69" s="15" t="inlineStr">
         <is>
           <t>Both</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Avg</t>
         </is>
       </c>
     </row>
@@ -12684,6 +12911,9 @@
           <t>NS</t>
         </is>
       </c>
+      <c r="J70" t="n">
+        <v>610</v>
+      </c>
     </row>
     <row r="71">
       <c r="B71" s="19" t="n"/>
@@ -12700,7 +12930,9 @@
       <c r="G71" s="7" t="n"/>
       <c r="H71" s="7" t="n"/>
       <c r="I71" s="7" t="n"/>
-      <c r="J71" s="7" t="n"/>
+      <c r="J71" s="7" t="n">
+        <v>560</v>
+      </c>
       <c r="K71" s="7" t="n"/>
     </row>
     <row r="72">
@@ -12720,6 +12952,9 @@
         <is>
           <t>Both</t>
         </is>
+      </c>
+      <c r="J72" t="n">
+        <v>460</v>
       </c>
     </row>
     <row r="73">
@@ -12734,6 +12969,16 @@
           <t>None</t>
         </is>
       </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="B74" s="19" t="n"/>
@@ -12750,7 +12995,9 @@
       <c r="G74" s="7" t="n"/>
       <c r="H74" s="7" t="n"/>
       <c r="I74" s="7" t="n"/>
-      <c r="J74" s="7" t="n"/>
+      <c r="J74" s="7" t="n">
+        <v>800</v>
+      </c>
       <c r="K74" s="7" t="n"/>
     </row>
     <row r="75">
@@ -12769,6 +13016,16 @@
       <c r="F75" s="15" t="inlineStr">
         <is>
           <t>Both</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Avg</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Avg</t>
         </is>
       </c>
     </row>
@@ -12783,6 +13040,9 @@
         <is>
           <t>None</t>
         </is>
+      </c>
+      <c r="J76" t="n">
+        <v>260</v>
       </c>
     </row>
     <row r="77">
@@ -12802,7 +13062,9 @@
       <c r="H77" s="7" t="n"/>
       <c r="I77" s="7" t="n"/>
       <c r="J77" s="7" t="n"/>
-      <c r="K77" s="7" t="n"/>
+      <c r="K77" s="7" t="n">
+        <v>780</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>